<commit_message>
Ajuste na formatação do arquivo
</commit_message>
<xml_diff>
--- a/OrcamentosIfc/OrcamentosIfc/OrcamentosIfc.xlsx
+++ b/OrcamentosIfc/OrcamentosIfc/OrcamentosIfc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\TCC\OrcamentosIfc\OrcamentosIfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3AF13D-8A76-445A-B1AD-BEA6EB9E269B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12A3EF3-122E-461E-91F7-C93866693E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4403AE4F-EC29-409D-ADA2-E6D08D35194D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="43" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Rótulos de Linha</t>
   </si>
@@ -103,6 +103,9 @@
   <si>
     <t>(vazio)</t>
   </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
@@ -140,21 +143,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -213,6 +283,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.0728305188266708E-3"/>
+          <c:y val="4.2872439975208251E-3"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -412,6 +490,80 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -428,7 +580,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>Custo Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -535,10 +687,137 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="930701503"/>
         <c:axId val="919780943"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabelas Dinâmicas'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tabelas Dinâmicas'!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(vazio)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabelas Dinâmicas'!$G$3:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E551-4E69-9276-1BD34B6E9392}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="588801120"/>
+        <c:axId val="1278578192"/>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="930701503"/>
         <c:scaling>
@@ -646,6 +925,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="1278578192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-9999"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588801120"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="588801120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1278578192"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2739,14 +3076,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Leonardo Rossi" refreshedDate="45253.865800810185" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{CA54AD04-D869-482B-9205-F42B490BEC47}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Leonardo Rossi" refreshedDate="45256.921263888886" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{CA54AD04-D869-482B-9205-F42B490BEC47}">
   <cacheSource type="worksheet">
     <worksheetSource name="tbDADOS"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Tipo" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="4">
+      <sharedItems containsNonDate="0" containsBlank="1" count="5">
         <m/>
+        <s v="Composicão" u="1"/>
         <s v="Insumo" u="1"/>
         <s v="Composição Análitica" u="1"/>
         <s v="Composição Sintética" u="1"/>
@@ -2756,8 +3094,11 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Nome Elemento" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="6">
+      <sharedItems containsNonDate="0" containsBlank="1" count="9">
         <m/>
+        <s v="PAREDE EXTERNA" u="1"/>
+        <s v="Tijolo, Comum" u="1"/>
+        <s v="PORCELANATO" u="1"/>
         <s v="Gesso" u="1"/>
         <s v="Embosso" u="1"/>
         <s v="Parede-004" u="1"/>
@@ -2766,8 +3107,11 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Descrição Item Sinapi" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="7">
+      <sharedItems containsNonDate="0" containsBlank="1" count="10">
         <m/>
+        <s v="ALVENARIA DE VEDAÇÃO DE BLOCOS CERÂMICOS FURADOS NA VERTICAL DE 19X19X39 CM (ESPESSURA 19 CM) E ARGAMASSA DE ASSENTAMENTO COM PREPARO EM BETONEIRA. AF_12/2021" u="1"/>
+        <s v="ALVENARIA DE VEDAÇÃO DE BLOCOS CERÂMICOS FURADOS NA HORIZONTAL DE 14X9X19 CM (ESPESSURA 14 CM, BLOCO DEITADO) E ARGAMASSA DE ASSENTAMENTO COM PREPARO EM BETONEIRA. AF_12/2021" u="1"/>
+        <s v="REVESTIMENTO CERÂMICO PARA PISO COM PLACAS TIPO PORCELANATO DE DIMENSÕES 60X60 CM APLICADA EM AMBIENTES DE ÁREA MAIOR QUE 10 M². AF_02/2023_PE" u="1"/>
         <s v="PASTILHEIRO (MENSALISTA)" u="1"/>
         <s v="PATCH CORD (CABO DE REDE), CATEGORIA 5 E (CAT 5E) UTP, 24 AWG, 4 PARES, EXTENSAO DE 1,50 M" u="1"/>
         <s v="CHAPISCO APLICADO EM ALVENARIAS E ESTRUTURAS DE CONCRETO INTERNAS, COM COLHER DE PEDREIRO.  ARGAMASSA TRAÇO 1:3 COM PREPARO EM BETONEIRA 400L. AF_10/2022" u="1"/>
@@ -2779,9 +3123,9 @@
     <cacheField name="Unidade" numFmtId="0">
       <sharedItems containsNonDate="0" containsBlank="1" count="4">
         <m/>
+        <s v="M2" u="1"/>
         <s v="MES   " u="1"/>
         <s v="UN    " u="1"/>
-        <s v="M2" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Dimensão Associada" numFmtId="0">
@@ -2825,47 +3169,217 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{786239AC-0410-45A6-8702-FEA41F16EDE1}" name="Tabela dinâmica3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F8F2389-5621-4A9B-A420-5803D9705314}" name="Tabela dinâmica2" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="E2:G4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
-      <items count="5">
+      <items count="6">
+        <item m="1" x="1"/>
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="10">
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item m="1" x="7"/>
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="1"/>
         <item m="1" x="2"/>
         <item m="1" x="3"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="11">
+        <item m="1" x="7"/>
+        <item m="1" x="2"/>
+        <item m="1" x="1"/>
+        <item m="1" x="9"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item m="1" x="1"/>
+        <item m="1" x="2"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
         <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField name="Preço Total2" dataField="1" numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Custo Total" fld="8" baseField="2" baseItem="0" numFmtId="41"/>
+    <dataField name="%" fld="8" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="9"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="3">
+    <chartFormat chart="7" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{786239AC-0410-45A6-8702-FEA41F16EDE1}" name="Tabela dinâmica3" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
     <pivotField showAll="0">
-      <items count="7">
-        <item m="1" x="2"/>
+      <items count="6">
         <item m="1" x="1"/>
         <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="10">
         <item m="1" x="5"/>
         <item m="1" x="4"/>
+        <item m="1" x="1"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item m="1" x="7"/>
+        <item m="1" x="3"/>
+        <item m="1" x="2"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="8">
+      <items count="11">
+        <item m="1" x="7"/>
+        <item m="1" x="9"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
         <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="3"/>
         <item m="1" x="5"/>
+        <item x="0"/>
         <item m="1" x="1"/>
         <item m="1" x="2"/>
-        <item x="0"/>
+        <item m="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0">
       <items count="5">
-        <item m="1" x="3"/>
         <item m="1" x="1"/>
         <item m="1" x="2"/>
+        <item m="1" x="3"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -2957,48 +3471,55 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CDEFFE8-3263-40F9-868C-39FD3D3FF5A2}" name="Tabela dinâmica1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CDEFFE8-3263-40F9-868C-39FD3D3FF5A2}" name="Tabela dinâmica1" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B2:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="9">
     <pivotField showAll="0">
-      <items count="5">
+      <items count="6">
+        <item m="1" x="1"/>
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
         <item m="1" x="2"/>
-        <item m="1" x="3"/>
-        <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="7">
-        <item m="1" x="2"/>
-        <item m="1" x="1"/>
-        <item m="1" x="3"/>
+      <items count="10">
         <item m="1" x="5"/>
         <item m="1" x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="8">
-        <item m="1" x="4"/>
+        <item m="1" x="1"/>
         <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item m="1" x="7"/>
         <item m="1" x="3"/>
-        <item m="1" x="5"/>
-        <item m="1" x="1"/>
         <item m="1" x="2"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0">
+      <items count="11">
+        <item m="1" x="7"/>
+        <item m="1" x="2"/>
+        <item m="1" x="1"/>
+        <item m="1" x="9"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
       <items count="5">
-        <item m="1" x="3"/>
         <item m="1" x="1"/>
         <item m="1" x="2"/>
+        <item m="1" x="3"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -3046,103 +3567,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F8F2389-5621-4A9B-A420-5803D9705314}" name="Tabela dinâmica2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="E2:F4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0">
-      <items count="5">
-        <item m="1" x="2"/>
-        <item m="1" x="3"/>
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item m="1" x="3"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item x="0"/>
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="8">
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="3"/>
-        <item m="1" x="5"/>
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField name="Preço Total2" dataField="1" numFmtId="3" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Custo Total" fld="8" baseField="2" baseItem="0" numFmtId="41"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="7" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Tipo" xr10:uid="{00DC8020-18C4-4664-9389-EBF642FCCE89}" sourceName="Tipo">
   <pivotTables>
@@ -3152,10 +3576,11 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="1482968320">
-      <items count="4">
+      <items count="5">
+        <i x="1" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
+        <i x="4" s="1" nd="1"/>
         <i x="2" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
         <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
@@ -3177,13 +3602,16 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="1482968320">
-      <items count="7">
+      <items count="10">
+        <i x="7" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
+        <i x="8" s="1" nd="1"/>
         <i x="4" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
+        <i x="5" s="1" nd="1"/>
         <i x="3" s="1" nd="1"/>
-        <i x="5" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
-        <i x="2" s="1" nd="1"/>
         <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
@@ -3206,9 +3634,9 @@
   <data>
     <tabular pivotCacheId="1482968320">
       <items count="4">
-        <i x="3" s="1" nd="1"/>
         <i x="1" s="1" nd="1"/>
         <i x="2" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
         <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
@@ -3253,12 +3681,15 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="1482968320">
-      <items count="6">
-        <i x="2" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
+      <items count="9">
         <i x="5" s="1" nd="1"/>
         <i x="4" s="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
+        <i x="8" s="1" nd="1"/>
+        <i x="7" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
         <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
@@ -3282,20 +3713,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF69A9A7-AA58-48F8-9546-0256C6B7151C}" name="tbDADOS" displayName="tbDADOS" ref="A1:I2" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF69A9A7-AA58-48F8-9546-0256C6B7151C}" name="tbDADOS" displayName="tbDADOS" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:I2" xr:uid="{BF69A9A7-AA58-48F8-9546-0256C6B7151C}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{15529957-7FE2-404C-8796-8CCD75DEB9B8}" name="Tipo"/>
-    <tableColumn id="2" xr3:uid="{641B7E46-AE61-4FC9-862B-6DFFC30E19D0}" name="Nome Projeto"/>
-    <tableColumn id="3" xr3:uid="{EEB783F8-D8FF-4366-8611-152C55D969A3}" name="Nome Elemento"/>
-    <tableColumn id="4" xr3:uid="{17ECFD7B-FB69-4005-BC14-5A3429C91C88}" name="Descrição Item Sinapi"/>
-    <tableColumn id="5" xr3:uid="{220C6397-C6D8-4A1C-88D4-B1744F097F93}" name="Unidade"/>
-    <tableColumn id="6" xr3:uid="{1527D8EB-F408-44A2-ABCE-5C689332BF9B}" name="Dimensão Associada"/>
-    <tableColumn id="7" xr3:uid="{BA60D4DE-DE82-456F-8042-4D8B2C69CF56}" name="Quantidade"/>
-    <tableColumn id="8" xr3:uid="{9456685B-D8D3-4C23-B8D4-C07727775115}" name="Preço Unitário"/>
-    <tableColumn id="9" xr3:uid="{E3A0DD8D-8E81-42E3-89B5-FCE61BAC2C45}" name="Preço Total" dataDxfId="0">
-      <calculatedColumnFormula>tbDADOS[[#This Row],[Quantidade]]*tbDADOS[[#This Row],[Preço Unitário]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{15529957-7FE2-404C-8796-8CCD75DEB9B8}" name="Tipo" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{641B7E46-AE61-4FC9-862B-6DFFC30E19D0}" name="Nome Projeto" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{EEB783F8-D8FF-4366-8611-152C55D969A3}" name="Nome Elemento" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{17ECFD7B-FB69-4005-BC14-5A3429C91C88}" name="Descrição Item Sinapi" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{220C6397-C6D8-4A1C-88D4-B1744F097F93}" name="Unidade" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{1527D8EB-F408-44A2-ABCE-5C689332BF9B}" name="Dimensão Associada" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{BA60D4DE-DE82-456F-8042-4D8B2C69CF56}" name="Quantidade" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{9456685B-D8D3-4C23-B8D4-C07727775115}" name="Preço Unitário" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{E3A0DD8D-8E81-42E3-89B5-FCE61BAC2C45}" name="Preço Total" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3599,7 +4028,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773BBEEE-77DF-4121-BA48-1B312B782A2E}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:DZ356"/>
+  <dimension ref="A1:DZ362"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
@@ -3612,362 +4041,368 @@
     <col min="131" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" customFormat="1" ht="9.9499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="358" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="359" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="360" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="361" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="362" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3984,57 +4419,66 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0041B8EA-2765-4953-BA47-09A41F040920}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="94.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="17" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
+      <c r="I2" s="6"/>
     </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="30" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="30" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -4048,8 +4492,8 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="B2:J4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4502,7 @@
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4067,13 +4511,16 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
@@ -4081,25 +4528,31 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="I3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="I4" s="3" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>